<commit_message>
Pushing some files from the last couple days.
</commit_message>
<xml_diff>
--- a/Early March/P4/p4_attribs.xlsx
+++ b/Early March/P4/p4_attribs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="240" windowWidth="23800" windowHeight="15320" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="240" windowWidth="13460" windowHeight="15320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -466,7 +466,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -486,6 +486,22 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -581,10 +597,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -629,8 +657,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -962,19 +1003,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="9" max="9" width="10.83203125" style="7"/>
-    <col min="10" max="16" width="10.83203125" style="8"/>
-    <col min="17" max="17" width="10.83203125" style="9"/>
-    <col min="18" max="18" width="10.83203125" style="11"/>
-    <col min="19" max="19" width="10.83203125" style="7"/>
-    <col min="20" max="21" width="10.83203125" style="8"/>
-    <col min="22" max="22" width="10.83203125" style="9"/>
+    <col min="3" max="8" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="7" customWidth="1"/>
+    <col min="10" max="16" width="10.83203125" style="8" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="9" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" style="11" customWidth="1"/>
+    <col min="19" max="19" width="10.83203125" style="7" customWidth="1"/>
+    <col min="20" max="21" width="10.83203125" style="8" customWidth="1"/>
+    <col min="22" max="22" width="10.83203125" style="9" customWidth="1"/>
     <col min="23" max="24" width="10.83203125" style="8"/>
     <col min="25" max="25" width="10.83203125" style="9"/>
   </cols>
@@ -1093,6 +1135,12 @@
       <c r="V2" s="9">
         <v>4</v>
       </c>
+      <c r="W2" s="18">
+        <v>1</v>
+      </c>
+      <c r="X2" s="18">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:25">
       <c r="A3">
@@ -1130,6 +1178,12 @@
       </c>
       <c r="V3" s="9">
         <v>3</v>
+      </c>
+      <c r="W3" s="18">
+        <v>2</v>
+      </c>
+      <c r="X3" s="18">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -1172,6 +1226,12 @@
       <c r="V4" s="9">
         <v>5</v>
       </c>
+      <c r="W4" s="18">
+        <v>3</v>
+      </c>
+      <c r="X4" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:25">
       <c r="A5">
@@ -1210,6 +1270,12 @@
       <c r="V5" s="9">
         <v>2</v>
       </c>
+      <c r="W5" s="18">
+        <v>4</v>
+      </c>
+      <c r="X5" s="18">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:25">
       <c r="A6">
@@ -1251,6 +1317,12 @@
       <c r="V6" s="9">
         <v>4</v>
       </c>
+      <c r="W6" s="18">
+        <v>5</v>
+      </c>
+      <c r="X6" s="18">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:25">
       <c r="A7">
@@ -1292,6 +1364,12 @@
       <c r="V7" s="9">
         <v>3</v>
       </c>
+      <c r="W7" s="18">
+        <v>3</v>
+      </c>
+      <c r="X7" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8">
@@ -1330,6 +1408,12 @@
       <c r="V8" s="9">
         <v>4</v>
       </c>
+      <c r="W8" s="18">
+        <v>1</v>
+      </c>
+      <c r="X8" s="18">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:25">
       <c r="A9">
@@ -1368,6 +1452,12 @@
       <c r="V9" s="9">
         <v>4</v>
       </c>
+      <c r="W9" s="18">
+        <v>5</v>
+      </c>
+      <c r="X9" s="18">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:25">
       <c r="A10">
@@ -1409,6 +1499,12 @@
       <c r="V10" s="9">
         <v>5</v>
       </c>
+      <c r="W10" s="18">
+        <v>2</v>
+      </c>
+      <c r="X10" s="18">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:25">
       <c r="A11">
@@ -1450,6 +1546,12 @@
       <c r="V11" s="9">
         <v>2</v>
       </c>
+      <c r="W11" s="18">
+        <v>3</v>
+      </c>
+      <c r="X11" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:25">
       <c r="A12">
@@ -1491,6 +1593,12 @@
       <c r="V12" s="9">
         <v>4</v>
       </c>
+      <c r="W12" s="18">
+        <v>1</v>
+      </c>
+      <c r="X12" s="18">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:25">
       <c r="A13">
@@ -1532,6 +1640,12 @@
       <c r="V13" s="9">
         <v>2</v>
       </c>
+      <c r="W13" s="18">
+        <v>2</v>
+      </c>
+      <c r="X13" s="18">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:25">
       <c r="A14">
@@ -1576,6 +1690,12 @@
       <c r="V14" s="9">
         <v>4</v>
       </c>
+      <c r="W14" s="18">
+        <v>1</v>
+      </c>
+      <c r="X14" s="18">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:25">
       <c r="A15">
@@ -1617,6 +1737,12 @@
       <c r="V15" s="9">
         <v>3</v>
       </c>
+      <c r="W15" s="18">
+        <v>4</v>
+      </c>
+      <c r="X15" s="18">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:25">
       <c r="A16">
@@ -1658,8 +1784,14 @@
       <c r="V16" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:22">
+      <c r="W16" s="18">
+        <v>3</v>
+      </c>
+      <c r="X16" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1708,8 +1840,14 @@
       <c r="V17" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:22">
+      <c r="W17" s="18">
+        <v>3</v>
+      </c>
+      <c r="X17" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1752,8 +1890,14 @@
       <c r="V18" s="9">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:22">
+      <c r="W18" s="18">
+        <v>3</v>
+      </c>
+      <c r="X18" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1796,8 +1940,14 @@
       <c r="V19" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:22">
+      <c r="W19" s="18">
+        <v>1</v>
+      </c>
+      <c r="X19" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1834,8 +1984,14 @@
       <c r="V20" s="9">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:22">
+      <c r="W20" s="18">
+        <v>3</v>
+      </c>
+      <c r="X20" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1884,8 +2040,14 @@
       <c r="V21" s="9">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:22">
+      <c r="W21" s="18">
+        <v>1</v>
+      </c>
+      <c r="X21" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1934,8 +2096,14 @@
       <c r="V22" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:22">
+      <c r="W22" s="18">
+        <v>3</v>
+      </c>
+      <c r="X22" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1981,8 +2149,14 @@
       <c r="V23" s="9">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:22">
+      <c r="W23" s="18">
+        <v>4</v>
+      </c>
+      <c r="X23" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2025,8 +2199,14 @@
       <c r="V24" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:22">
+      <c r="W24" s="18">
+        <v>3</v>
+      </c>
+      <c r="X24" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2066,8 +2246,14 @@
       <c r="V25" s="9">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:22">
+      <c r="W25" s="18">
+        <v>1</v>
+      </c>
+      <c r="X25" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2104,8 +2290,14 @@
       <c r="V26" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:22">
+      <c r="W26" s="18">
+        <v>2</v>
+      </c>
+      <c r="X26" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2151,9 +2343,16 @@
       <c r="V27" s="9">
         <v>4</v>
       </c>
+      <c r="W27" s="18">
+        <v>5</v>
+      </c>
+      <c r="X27" s="18">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>